<commit_message>
update table with caption
</commit_message>
<xml_diff>
--- a/tables/table1.xlsx
+++ b/tables/table1.xlsx
@@ -1,23 +1,18 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22827"/>
-  <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\שקד סלובין\Desktop\TIGEM_lab\reviwe\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3C3169AD-638E-45CA-BDA1-63075AED566D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="7" rupBuild="4506"/>
+  <workbookPr/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" xr2:uid="{4B860663-E72D-4F85-B593-2CD9F71460B4}"/>
+    <workbookView xWindow="-105" yWindow="-105" windowWidth="19425" windowHeight="11025"/>
   </bookViews>
   <sheets>
-    <sheet name="גיליון1" sheetId="1" r:id="rId1"/>
+    <sheet name="caption" sheetId="2" r:id="rId1"/>
+    <sheet name="Table 1" sheetId="1" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="181029"/>
-  <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+  <calcPr calcId="125725"/>
+  <extLst xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main">
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -31,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="34">
   <si>
     <t>Method</t>
   </si>
@@ -130,19 +125,50 @@
   </si>
   <si>
     <t>[99]</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Table 1 - scRNA-seq technologies and their relative costs.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="177"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">  For each scRNA-seq technology reported are: the category it belongs, the transcript coverage, its sensitivity and the relative cost per cell that range from + (i.e. cheap) to +++ (i.e. expensive).</t>
+    </r>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="6">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="177"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -167,16 +193,36 @@
       <charset val="177"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.14999847407452621"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="2">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -199,36 +245,77 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" indent="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1" indent="2"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="3" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" indent="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1" indent="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="היפר-קישור" xfId="1" builtinId="8"/>
+    <cellStyle name="Collegamento ipertestuale" xfId="1" builtinId="8"/>
+    <cellStyle name="Normale" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -286,7 +373,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック Light"/>
@@ -338,7 +425,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック"/>
@@ -532,224 +619,297 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B95F8AD5-6C95-47A4-9DE9-49BDD9BFED39}">
-  <dimension ref="A1:I9"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="G4" sqref="G4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D40" sqref="D40"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="7" max="7" width="56.6328125" customWidth="1"/>
+    <col min="1" max="1" width="65.875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="62" x14ac:dyDescent="0.35">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:1" ht="46.5" customHeight="1">
+      <c r="A1" s="12" t="s">
+        <v>33</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:J13"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C16" sqref="C16"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="2" max="2" width="17.625" customWidth="1"/>
+    <col min="3" max="3" width="14.625" customWidth="1"/>
+    <col min="4" max="4" width="20" customWidth="1"/>
+    <col min="5" max="5" width="27.625" customWidth="1"/>
+    <col min="6" max="6" width="6.375" customWidth="1"/>
+    <col min="7" max="7" width="5.875" customWidth="1"/>
+    <col min="8" max="8" width="7.625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10">
+      <c r="A1" s="7"/>
+      <c r="B1" s="7"/>
+      <c r="C1" s="7"/>
+      <c r="D1" s="7"/>
+      <c r="E1" s="7"/>
+      <c r="F1" s="7"/>
+      <c r="G1" s="7"/>
+      <c r="H1" s="7"/>
+    </row>
+    <row r="2" spans="1:10" ht="16.5" thickBot="1">
+      <c r="A2" s="7"/>
+      <c r="B2" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="C2" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D2" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E2" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F2" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G2" s="2" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="2" spans="1:9" ht="77.5" x14ac:dyDescent="0.35">
-      <c r="A2" s="2" t="s">
+      <c r="H2" s="7"/>
+    </row>
+    <row r="3" spans="1:10" ht="30">
+      <c r="A3" s="7"/>
+      <c r="B3" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="C3" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="D3" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="E3" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="E2" s="2" t="s">
+      <c r="F3" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="F2" s="3" t="s">
+      <c r="G3" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="G2" s="6"/>
-    </row>
-    <row r="3" spans="1:9" ht="77.5" x14ac:dyDescent="0.35">
-      <c r="A3" s="2" t="s">
+      <c r="H3" s="8"/>
+    </row>
+    <row r="4" spans="1:10" ht="30">
+      <c r="A4" s="7"/>
+      <c r="B4" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="B3" s="2" t="s">
+      <c r="C4" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="C3" s="2" t="s">
+      <c r="D4" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="D3" s="2" t="s">
+      <c r="E4" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="E3" s="2" t="s">
+      <c r="F4" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="F3" s="3" t="s">
+      <c r="G4" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="G3" s="7"/>
-    </row>
-    <row r="4" spans="1:9" ht="77.5" x14ac:dyDescent="0.35">
-      <c r="A4" s="2" t="s">
+      <c r="H4" s="9"/>
+    </row>
+    <row r="5" spans="1:10" ht="30">
+      <c r="A5" s="7"/>
+      <c r="B5" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="B4" s="2" t="s">
+      <c r="C5" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="C4" s="2" t="s">
+      <c r="D5" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="D4" s="2" t="s">
+      <c r="E5" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="E4" s="2" t="s">
+      <c r="F5" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="F4" s="3" t="s">
+      <c r="G5" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="G4" s="7"/>
-    </row>
-    <row r="5" spans="1:9" ht="93" x14ac:dyDescent="0.35">
-      <c r="A5" s="2" t="s">
+      <c r="H5" s="9"/>
+    </row>
+    <row r="6" spans="1:10" ht="30">
+      <c r="A6" s="7"/>
+      <c r="B6" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="B5" s="2" t="s">
+      <c r="C6" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="C5" s="2" t="s">
+      <c r="D6" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="D5" s="2" t="s">
+      <c r="E6" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="E5" s="2" t="s">
+      <c r="F6" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="F5" s="3" t="s">
+      <c r="G6" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="G5" s="4"/>
-    </row>
-    <row r="6" spans="1:9" ht="93" x14ac:dyDescent="0.35">
-      <c r="A6" s="2" t="s">
+      <c r="H6" s="10"/>
+    </row>
+    <row r="7" spans="1:10" ht="30">
+      <c r="A7" s="7"/>
+      <c r="B7" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="B6" s="2" t="s">
+      <c r="C7" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="C6" s="2" t="s">
+      <c r="D7" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="D6" s="2" t="s">
+      <c r="E7" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="E6" s="2" t="s">
+      <c r="F7" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="F6" s="3" t="s">
+      <c r="G7" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="G6" s="4"/>
-    </row>
-    <row r="7" spans="1:9" ht="93" x14ac:dyDescent="0.35">
-      <c r="A7" s="2" t="s">
+      <c r="H7" s="10"/>
+    </row>
+    <row r="8" spans="1:10" ht="30">
+      <c r="A8" s="7"/>
+      <c r="B8" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="B7" s="2" t="s">
+      <c r="C8" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="C7" s="2" t="s">
+      <c r="D8" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="D7" s="2" t="s">
+      <c r="E8" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="E7" s="2" t="s">
+      <c r="F8" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="F7" s="3" t="s">
+      <c r="G8" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="G7" s="5"/>
-      <c r="I7" s="6"/>
-    </row>
-    <row r="8" spans="1:9" ht="93" x14ac:dyDescent="0.35">
-      <c r="A8" s="2" t="s">
+      <c r="H8" s="11"/>
+      <c r="J8" s="1"/>
+    </row>
+    <row r="9" spans="1:10" ht="30">
+      <c r="A9" s="7"/>
+      <c r="B9" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="B8" s="2" t="s">
+      <c r="C9" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="C8" s="2" t="s">
+      <c r="D9" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="D8" s="2" t="s">
+      <c r="E9" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="E8" s="2" t="s">
+      <c r="F9" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="F8" s="3" t="s">
+      <c r="G9" s="6" t="s">
         <v>30</v>
       </c>
-      <c r="G8" s="7"/>
-    </row>
-    <row r="9" spans="1:9" ht="93" x14ac:dyDescent="0.35">
-      <c r="A9" s="2" t="s">
+      <c r="H9" s="9"/>
+    </row>
+    <row r="10" spans="1:10" ht="30">
+      <c r="A10" s="7"/>
+      <c r="B10" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="B9" s="2" t="s">
+      <c r="C10" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="C9" s="2" t="s">
+      <c r="D10" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="D9" s="2" t="s">
+      <c r="E10" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="E9" s="2" t="s">
+      <c r="F10" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="F9" s="3" t="s">
+      <c r="G10" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="G9" s="4"/>
+      <c r="H10" s="10"/>
+    </row>
+    <row r="11" spans="1:10">
+      <c r="A11" s="7"/>
+      <c r="B11" s="7"/>
+      <c r="C11" s="7"/>
+      <c r="D11" s="7"/>
+      <c r="E11" s="7"/>
+      <c r="F11" s="7"/>
+      <c r="G11" s="7"/>
+      <c r="H11" s="7"/>
+    </row>
+    <row r="12" spans="1:10">
+      <c r="A12" s="7"/>
+      <c r="B12" s="7"/>
+      <c r="C12" s="7"/>
+      <c r="D12" s="7"/>
+      <c r="E12" s="7"/>
+      <c r="F12" s="7"/>
+      <c r="G12" s="7"/>
+      <c r="H12" s="7"/>
+    </row>
+    <row r="13" spans="1:10">
+      <c r="A13" s="7"/>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="F2" r:id="rId1" display="https://paperpile.com/c/RHRBs0/fCl3w" xr:uid="{262CFBAF-D8D4-429B-A919-9F9821910075}"/>
-    <hyperlink ref="F3" r:id="rId2" display="https://paperpile.com/c/RHRBs0/H2g5Q" xr:uid="{B6AE90C0-3568-4100-A9B0-9AC30A3FAEA3}"/>
-    <hyperlink ref="F4" r:id="rId3" display="https://paperpile.com/c/RHRBs0/A5TIB" xr:uid="{418F2924-0B52-4A01-B343-4426C56AC9FC}"/>
-    <hyperlink ref="F5" r:id="rId4" display="https://paperpile.com/c/RHRBs0/jpUg2" xr:uid="{AF9D62BA-96F0-40E1-BF56-223A3945E342}"/>
-    <hyperlink ref="F6" r:id="rId5" display="https://paperpile.com/c/RHRBs0/ihGtf" xr:uid="{AEE96590-36E8-49C6-899D-2EA3218D4D5F}"/>
-    <hyperlink ref="F7" r:id="rId6" display="https://paperpile.com/c/RHRBs0/z8dhG+XayWy" xr:uid="{8456E5FD-D69C-40D2-BA94-4BFE0C76393C}"/>
-    <hyperlink ref="F8" r:id="rId7" display="https://paperpile.com/c/RHRBs0/szx8B" xr:uid="{A3CC2128-9EA2-4BDF-996A-7E5125BD4811}"/>
-    <hyperlink ref="F9" r:id="rId8" display="https://paperpile.com/c/RHRBs0/VvYHQ" xr:uid="{6CDFA338-D94B-4B5A-BEED-E73034A194EA}"/>
+    <hyperlink ref="G3" r:id="rId1" display="https://paperpile.com/c/RHRBs0/fCl3w"/>
+    <hyperlink ref="G4" r:id="rId2" display="https://paperpile.com/c/RHRBs0/H2g5Q"/>
+    <hyperlink ref="G5" r:id="rId3" display="https://paperpile.com/c/RHRBs0/A5TIB"/>
+    <hyperlink ref="G6" r:id="rId4" display="https://paperpile.com/c/RHRBs0/jpUg2"/>
+    <hyperlink ref="G7" r:id="rId5" display="https://paperpile.com/c/RHRBs0/ihGtf"/>
+    <hyperlink ref="G8" r:id="rId6" display="https://paperpile.com/c/RHRBs0/z8dhG+XayWy"/>
+    <hyperlink ref="G9" r:id="rId7" display="https://paperpile.com/c/RHRBs0/szx8B"/>
+    <hyperlink ref="G10" r:id="rId8" display="https://paperpile.com/c/RHRBs0/VvYHQ"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>